<commit_message>
adding nefarious new data
</commit_message>
<xml_diff>
--- a/src/data-cleaning/data_received/data_20240120.xlsx
+++ b/src/data-cleaning/data_received/data_20240120.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgaythor\Documents\Teaching\orderly_training\src\A-data-cleaning\data_received\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgaythor\Documents\Teaching\orderly_training\src\data-cleaning\data_received\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B6F2E7-3945-4547-9740-26867A852A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3C933C8-87C5-4BC6-ABFF-3A6A65FFC1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{5273AEA4-57F6-43AA-8CCA-05F0B2D92416}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5273AEA4-57F6-43AA-8CCA-05F0B2D92416}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -507,9 +507,9 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -521,7 +521,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -535,7 +535,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="4" t="s">
         <v>1</v>
@@ -549,7 +549,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="4" t="s">
         <v>2</v>
@@ -563,7 +563,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -575,7 +575,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="4" t="s">
         <v>3</v>
@@ -589,7 +589,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -617,22 +617,22 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -643,7 +643,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -654,7 +654,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -665,7 +665,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -676,7 +676,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -687,7 +687,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -698,7 +698,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -709,7 +709,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -720,7 +720,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -731,7 +731,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -742,7 +742,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -753,7 +753,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
@@ -764,7 +764,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -775,7 +775,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -786,7 +786,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -797,7 +797,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -808,7 +808,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
@@ -819,7 +819,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
@@ -830,7 +830,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>11</v>
       </c>
@@ -841,7 +841,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
@@ -852,7 +852,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -863,7 +863,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>8</v>
       </c>
@@ -874,7 +874,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -885,7 +885,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>6</v>
       </c>
@@ -899,5 +899,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>